<commit_message>
workflow works on its own but not integrated with Wanlin's datatables
</commit_message>
<xml_diff>
--- a/Singles Event Registration (Responses).xlsx
+++ b/Singles Event Registration (Responses).xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enaij\OneDrive - Nanyang Technological University\Documents\MSBA Materials\AN6817 - RPA\Projects\GroupAssg\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\3. RPA for Analytics\UIPath Projects\team5_RPAproject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA27A28-0E12-4D44-B3B3-08F60C393889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD275064-22DB-49FF-8ED8-D8E5C93486D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2832" yWindow="0" windowWidth="17280" windowHeight="16656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="345" yWindow="4005" windowWidth="15000" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form responses 1" sheetId="1" r:id="rId1"/>
@@ -502,16 +502,16 @@
   <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E65" sqref="E65"/>
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="12" width="18.88671875" customWidth="1"/>
+    <col min="1" max="12" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -531,7 +531,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>45417.834606481483</v>
       </c>
@@ -548,10 +548,10 @@
         <v>9</v>
       </c>
       <c r="F2" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>14583376</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>45418.152708333335</v>
       </c>
@@ -568,10 +568,10 @@
         <v>9</v>
       </c>
       <c r="F3" s="1">
-        <v>23456789</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>15480124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>45416.657222222224</v>
       </c>
@@ -588,10 +588,10 @@
         <v>9</v>
       </c>
       <c r="F4" s="1">
-        <v>12410597</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>19760685</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>45418.502638888887</v>
       </c>
@@ -608,10 +608,10 @@
         <v>9</v>
       </c>
       <c r="F5" s="1">
-        <v>34567890</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>22789443</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>45419.741041666668</v>
       </c>
@@ -628,10 +628,10 @@
         <v>9</v>
       </c>
       <c r="F6" s="1">
-        <v>45678901</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>24219363</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>45418.524965277778</v>
       </c>
@@ -648,10 +648,10 @@
         <v>9</v>
       </c>
       <c r="F7" s="1">
-        <v>41502917</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>24770454</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>45416.004884259259</v>
       </c>
@@ -668,10 +668,10 @@
         <v>9</v>
       </c>
       <c r="F8" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>26663693</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>45417.274467592593</v>
       </c>
@@ -688,10 +688,10 @@
         <v>9</v>
       </c>
       <c r="F9" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>27498330</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>45418.074513888889</v>
       </c>
@@ -708,10 +708,10 @@
         <v>9</v>
       </c>
       <c r="F10" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>28557906</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>45417.56521990741</v>
       </c>
@@ -728,10 +728,10 @@
         <v>9</v>
       </c>
       <c r="F11" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>28688027</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>45416.657222222224</v>
       </c>
@@ -748,10 +748,10 @@
         <v>9</v>
       </c>
       <c r="F12" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>30279019</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>45418.502638888887</v>
       </c>
@@ -768,10 +768,10 @@
         <v>24</v>
       </c>
       <c r="F13" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>30338111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>45419.741041666668</v>
       </c>
@@ -788,10 +788,10 @@
         <v>24</v>
       </c>
       <c r="F14" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>30990800</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>45418.524965277778</v>
       </c>
@@ -808,10 +808,10 @@
         <v>24</v>
       </c>
       <c r="F15" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+        <v>31310453</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>45416.004884259259</v>
       </c>
@@ -828,10 +828,10 @@
         <v>24</v>
       </c>
       <c r="F16" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+        <v>34344874</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>45417.274467592593</v>
       </c>
@@ -848,10 +848,10 @@
         <v>24</v>
       </c>
       <c r="F17" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+        <v>34650095</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>45418.074513888889</v>
       </c>
@@ -868,10 +868,10 @@
         <v>24</v>
       </c>
       <c r="F18" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+        <v>36373341</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>45417.56521990741</v>
       </c>
@@ -888,10 +888,10 @@
         <v>24</v>
       </c>
       <c r="F19" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+        <v>37105247</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>45418.524780092594</v>
       </c>
@@ -908,10 +908,10 @@
         <v>24</v>
       </c>
       <c r="F20" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+        <v>38559467</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>45419.872337962966</v>
       </c>
@@ -928,10 +928,10 @@
         <v>24</v>
       </c>
       <c r="F21" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+        <v>39467735</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>45419.29074074074</v>
       </c>
@@ -948,10 +948,10 @@
         <v>24</v>
       </c>
       <c r="F22" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+        <v>41370596</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>45418.899872685186</v>
       </c>
@@ -968,10 +968,10 @@
         <v>24</v>
       </c>
       <c r="F23" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+        <v>42487189</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>45417.960914351854</v>
       </c>
@@ -988,10 +988,10 @@
         <v>24</v>
       </c>
       <c r="F24" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+        <v>42910376</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>45417.62091435185</v>
       </c>
@@ -1008,10 +1008,10 @@
         <v>24</v>
       </c>
       <c r="F25" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+        <v>45345003</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>45417.076944444445</v>
       </c>
@@ -1028,10 +1028,10 @@
         <v>24</v>
       </c>
       <c r="F26" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+        <v>46587488</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>45419.049988425926</v>
       </c>
@@ -1048,10 +1048,10 @@
         <v>24</v>
       </c>
       <c r="F27" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+        <v>46935167</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>45416.204432870371</v>
       </c>
@@ -1068,10 +1068,10 @@
         <v>24</v>
       </c>
       <c r="F28" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+        <v>53195057</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>45418.421817129631</v>
       </c>
@@ -1088,10 +1088,10 @@
         <v>24</v>
       </c>
       <c r="F29" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+        <v>53416701</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>45416.983206018522</v>
       </c>
@@ -1108,10 +1108,10 @@
         <v>24</v>
       </c>
       <c r="F30" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+        <v>53596124</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>45417.145462962966</v>
       </c>
@@ -1128,10 +1128,10 @@
         <v>24</v>
       </c>
       <c r="F31" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+        <v>54076152</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>45419.701435185183</v>
       </c>
@@ -1148,10 +1148,10 @@
         <v>24</v>
       </c>
       <c r="F32" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+        <v>58574868</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>45419.654490740744</v>
       </c>
@@ -1168,10 +1168,10 @@
         <v>24</v>
       </c>
       <c r="F33" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+        <v>62193437</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>45416.639594907407</v>
       </c>
@@ -1188,10 +1188,10 @@
         <v>24</v>
       </c>
       <c r="F34" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+        <v>62283126</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>45419.332673611112</v>
       </c>
@@ -1208,10 +1208,10 @@
         <v>24</v>
       </c>
       <c r="F35" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+        <v>62798342</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>45416.013541666667</v>
       </c>
@@ -1228,10 +1228,10 @@
         <v>24</v>
       </c>
       <c r="F36" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+        <v>67424150</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>45416.033449074072</v>
       </c>
@@ -1248,10 +1248,10 @@
         <v>24</v>
       </c>
       <c r="F37" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+        <v>67431110</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>45418.474988425929</v>
       </c>
@@ -1268,10 +1268,10 @@
         <v>24</v>
       </c>
       <c r="F38" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+        <v>69526335</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>45416.582650462966</v>
       </c>
@@ -1288,10 +1288,10 @@
         <v>24</v>
       </c>
       <c r="F39" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+        <v>71034050</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>45419.117881944447</v>
       </c>
@@ -1308,10 +1308,10 @@
         <v>24</v>
       </c>
       <c r="F40" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+        <v>72696126</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>45417.270972222221</v>
       </c>
@@ -1328,10 +1328,10 @@
         <v>24</v>
       </c>
       <c r="F41" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+        <v>74719844</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>45419.140057870369</v>
       </c>
@@ -1348,10 +1348,10 @@
         <v>24</v>
       </c>
       <c r="F42" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+        <v>78475997</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>45416.110196759262</v>
       </c>
@@ -1368,10 +1368,10 @@
         <v>24</v>
       </c>
       <c r="F43" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+        <v>78668846</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>45417.91615740741</v>
       </c>
@@ -1388,10 +1388,10 @@
         <v>24</v>
       </c>
       <c r="F44" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+        <v>80699407</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>45417.773946759262</v>
       </c>
@@ -1408,10 +1408,10 @@
         <v>24</v>
       </c>
       <c r="F45" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+        <v>81218466</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>45417.699050925927</v>
       </c>
@@ -1428,10 +1428,10 @@
         <v>24</v>
       </c>
       <c r="F46" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+        <v>86347520</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>45419.132094907407</v>
       </c>
@@ -1448,10 +1448,10 @@
         <v>24</v>
       </c>
       <c r="F47" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+        <v>87857672</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>45416.43109953704</v>
       </c>
@@ -1468,10 +1468,10 @@
         <v>24</v>
       </c>
       <c r="F48" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+        <v>88062606</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>45419.133622685185</v>
       </c>
@@ -1488,10 +1488,10 @@
         <v>24</v>
       </c>
       <c r="F49" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+        <v>89431443</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>45416.009814814817</v>
       </c>
@@ -1508,10 +1508,10 @@
         <v>24</v>
       </c>
       <c r="F50" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+        <v>91762639</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>45416.406226851854</v>
       </c>
@@ -1528,10 +1528,10 @@
         <v>24</v>
       </c>
       <c r="F51" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+        <v>92312909</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>45418.010671296295</v>
       </c>
@@ -1548,10 +1548,10 @@
         <v>24</v>
       </c>
       <c r="F52" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+        <v>93038340</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>45416.752858796295</v>
       </c>
@@ -1568,10 +1568,10 @@
         <v>24</v>
       </c>
       <c r="F53" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+        <v>93268593</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>45418.247928240744</v>
       </c>
@@ -1588,10 +1588,10 @@
         <v>24</v>
       </c>
       <c r="F54" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+        <v>94192223</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>45418.00403935185</v>
       </c>
@@ -1608,10 +1608,10 @@
         <v>24</v>
       </c>
       <c r="F55" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+        <v>95425054</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>45417.710347222222</v>
       </c>
@@ -1628,10 +1628,10 @@
         <v>24</v>
       </c>
       <c r="F56" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+        <v>98427834</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>45419.996168981481</v>
       </c>
@@ -1648,22 +1648,22 @@
         <v>24</v>
       </c>
       <c r="F57" s="1">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+        <v>99338799</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
     </row>
-    <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D59" s="1"/>
     </row>
-    <row r="60" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D60" s="1"/>
     </row>
-    <row r="61" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D61" s="1"/>
     </row>
   </sheetData>

</xml_diff>